<commit_message>
improved reward function and fixed multiple bugs
</commit_message>
<xml_diff>
--- a/AI_GAME_2022/src/server/probabilities/1.xlsx
+++ b/AI_GAME_2022/src/server/probabilities/1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dars\TAs\AI2_TA\src\server\probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parisa\Desktop\AI-Phase2-fall2022\AI_GAME_2022\src\server\probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBE57CD-8E55-4EF5-9FD0-E105EF1EE080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84161CD-6EFC-4AFB-8BFA-A7C204E3A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="normal" sheetId="1" r:id="rId1"/>
@@ -381,12 +381,12 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.265625" defaultRowHeight="24.4" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -419,12 +419,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -454,7 +454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -559,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,7 +576,7 @@
         <v>0.1</v>
       </c>
       <c r="F6" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -629,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -747,9 +747,9 @@
       <selection activeCell="K1" sqref="K1:K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.46484375" defaultRowHeight="31.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="31.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -782,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="31.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1110,9 +1110,9 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="30.4" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="30.45" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="30.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1473,9 +1473,9 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>